<commit_message>
separate tables for wind and solar
</commit_message>
<xml_diff>
--- a/docs/_static/exclusion_parameters_overview.xlsx
+++ b/docs/_static/exclusion_parameters_overview.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GE\Faggrupper\LTES\Cross country projects 2025\LAVA-tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b396636\Documents\Turkiye_private\programming_turkiye\land_availability\docs\_static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{059CEDF9-B6B0-4905-955B-143B2BBA57D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D886D-8470-42BB-843E-4F7DA7616FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D1C09A3-EC3E-4F55-B1EC-A35F9EA6C094}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{8D1C09A3-EC3E-4F55-B1EC-A35F9EA6C094}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="onshorewind" sheetId="1" r:id="rId1"/>
+    <sheet name="solar PV ground" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>criteria</t>
   </si>
@@ -155,9 +156,6 @@
     <t>wind speed</t>
   </si>
   <si>
-    <t>worldpop</t>
-  </si>
-  <si>
     <t>OSM</t>
   </si>
   <si>
@@ -167,9 +165,6 @@
     <t>GWA</t>
   </si>
   <si>
-    <t>&lt;5</t>
-  </si>
-  <si>
     <t>pixels connected (filter)</t>
   </si>
   <si>
@@ -209,13 +204,34 @@
     <t>substations</t>
   </si>
   <si>
-    <t>copy table for multiple scenarios and distinguish between solar and wind</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>landcover (code)</t>
+  </si>
+  <si>
+    <t>scenario 1</t>
+  </si>
+  <si>
+    <t>scenario 2</t>
+  </si>
+  <si>
+    <t>&lt;3000m</t>
+  </si>
+  <si>
+    <t>&lt;100m &amp; &gt;10000m</t>
+  </si>
+  <si>
+    <t>residential areas</t>
+  </si>
+  <si>
+    <t>&lt;300m</t>
+  </si>
+  <si>
+    <t>WSF 2019</t>
+  </si>
+  <si>
+    <t>Worldpop (year)</t>
+  </si>
+  <si>
+    <t>&lt;100</t>
   </si>
 </sst>
 </file>
@@ -259,18 +275,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,345 +616,715 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18C1CA-23D3-47BC-BC83-CDCB1C3DDEFC}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D92FEE-935E-421C-95F5-75F49D715FF2}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" t="s">
-        <v>42</v>
+      <c r="B32" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F3"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
separate sheeet data sources
</commit_message>
<xml_diff>
--- a/docs/_static/exclusion_parameters_overview.xlsx
+++ b/docs/_static/exclusion_parameters_overview.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b396636\Documents\Turkiye_private\programming_turkiye\land_availability\docs\_static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D886D-8470-42BB-843E-4F7DA7616FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5389FD8D-57FF-42E5-BCFF-9C878E5AE6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{8D1C09A3-EC3E-4F55-B1EC-A35F9EA6C094}"/>
+    <workbookView xWindow="28680" yWindow="-315" windowWidth="29040" windowHeight="15720" xr2:uid="{8D1C09A3-EC3E-4F55-B1EC-A35F9EA6C094}"/>
   </bookViews>
   <sheets>
-    <sheet name="onshorewind" sheetId="1" r:id="rId1"/>
-    <sheet name="solar PV ground" sheetId="2" r:id="rId2"/>
+    <sheet name="data sources" sheetId="3" r:id="rId1"/>
+    <sheet name="onshorewind" sheetId="1" r:id="rId2"/>
+    <sheet name="solar PV ground" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
   <si>
     <t>criteria</t>
   </si>
@@ -54,9 +55,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>ESAworldcover</t>
-  </si>
-  <si>
     <t>Tree (10)</t>
   </si>
   <si>
@@ -198,9 +196,6 @@
     <t>WDPA</t>
   </si>
   <si>
-    <t>see below</t>
-  </si>
-  <si>
     <t>substations</t>
   </si>
   <si>
@@ -232,13 +227,55 @@
   </si>
   <si>
     <t>&lt;100</t>
+  </si>
+  <si>
+    <t>distribution lines</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>ESA_WORLDCOVER_10M_2021_V2</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>15 arcsec (463m @equator)</t>
+  </si>
+  <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>100m</t>
+  </si>
+  <si>
+    <t>30 arcsec (~1 km)</t>
+  </si>
+  <si>
+    <t>250m</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>PVOUT (kWh/kW/a)</t>
+  </si>
+  <si>
+    <t>wind speed @100m</t>
+  </si>
+  <si>
+    <t>actual DTM</t>
+  </si>
+  <si>
+    <t>not used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,13 +291,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,18 +329,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -615,80 +677,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18C1CA-23D3-47BC-BC83-CDCB1C3DDEFC}">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D31C76-1A8C-4B0E-AE4B-BACC3D2A9F3D}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D071E76A-CA52-41A0-A384-F19AC57A0B0C}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{D65E9C3A-1F86-43EA-8F2A-DDB67D1B7BF3}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{E8928AF7-5BD9-4484-921D-01DC3E921B47}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{3E840665-3C2E-4816-B118-F1DECECFD536}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{9A10D374-DFD4-43E5-942D-9058CD9EBFDE}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{6BE7D4DB-648A-445A-892D-9E8816FA8346}"/>
+    <hyperlink ref="B20" r:id="rId7" xr:uid="{0B617A10-23AA-4D90-8756-9D0680367E6B}"/>
+    <hyperlink ref="B19" r:id="rId8" xr:uid="{5AEB4E2A-2394-4A6D-A91F-B62BAFE90E18}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18C1CA-23D3-47BC-BC83-CDCB1C3DDEFC}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -696,357 +1022,291 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
       <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="D29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D92FEE-935E-421C-95F5-75F49D715FF2}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1054,278 +1314,520 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8C519A0C07EDA47BFE3C2D04A9A16E8" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5af8a87c7f5a09efbaa0de1bfbdabc53">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7" xmlns:ns3="730a4b66-01d8-4cde-8d8b-f146b54eaab0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d85c399567fc6e954f4786affeeee316" ns2:_="" ns3:_="">
+    <xsd:import namespace="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7"/>
+    <xsd:import namespace="730a4b66-01d8-4cde-8d8b-f146b54eaab0"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:_dlc_DocId" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdUrl" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdPersistId" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_dlc_DocId" ma:index="8" nillable="true" ma:displayName="Document ID Value" ma:description="The value of the document ID assigned to this item." ma:internalName="_dlc_DocId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdUrl" ma:index="9" nillable="true" ma:displayName="Document ID" ma:description="Permanent link to this document." ma:hidden="true" ma:internalName="_dlc_DocIdUrl" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdPersistId" ma:index="10" nillable="true" ma:displayName="Persist ID" ma:description="Keep ID on add." ma:hidden="true" ma:internalName="_dlc_DocIdPersistId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="730a4b66-01d8-4cde-8d8b-f146b54eaab0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7">GE00-939878155-298</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7">
+      <Url>https://sp.ens.dk/sites/gr/keny/_layouts/15/DocIdRedir.aspx?ID=GE00-939878155-298</Url>
+      <Description>GE00-939878155-298</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2FE42FC-3536-4A73-B9F7-AADAD56E28F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7"/>
+    <ds:schemaRef ds:uri="730a4b66-01d8-4cde-8d8b-f146b54eaab0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64FA2BBB-2582-437A-AF5D-6FFA5E5689E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{964EE766-D6F8-4013-8CB4-BEDD892B39AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD566AB5-C4C6-4641-BE27-5E6E12A6FDD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="730a4b66-01d8-4cde-8d8b-f146b54eaab0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated docs based on main repo from DEA-GE/LAVA
</commit_message>
<xml_diff>
--- a/docs/_static/exclusion_parameters_overview.xlsx
+++ b/docs/_static/exclusion_parameters_overview.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b396636\Documents\Turkiye_private\programming_turkiye\land_availability\docs\_static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D886D-8470-42BB-843E-4F7DA7616FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5389FD8D-57FF-42E5-BCFF-9C878E5AE6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{8D1C09A3-EC3E-4F55-B1EC-A35F9EA6C094}"/>
+    <workbookView xWindow="28680" yWindow="-315" windowWidth="29040" windowHeight="15720" xr2:uid="{8D1C09A3-EC3E-4F55-B1EC-A35F9EA6C094}"/>
   </bookViews>
   <sheets>
-    <sheet name="onshorewind" sheetId="1" r:id="rId1"/>
-    <sheet name="solar PV ground" sheetId="2" r:id="rId2"/>
+    <sheet name="data sources" sheetId="3" r:id="rId1"/>
+    <sheet name="onshorewind" sheetId="1" r:id="rId2"/>
+    <sheet name="solar PV ground" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
   <si>
     <t>criteria</t>
   </si>
@@ -54,9 +55,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>ESAworldcover</t>
-  </si>
-  <si>
     <t>Tree (10)</t>
   </si>
   <si>
@@ -198,9 +196,6 @@
     <t>WDPA</t>
   </si>
   <si>
-    <t>see below</t>
-  </si>
-  <si>
     <t>substations</t>
   </si>
   <si>
@@ -232,13 +227,55 @@
   </si>
   <si>
     <t>&lt;100</t>
+  </si>
+  <si>
+    <t>distribution lines</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>ESA_WORLDCOVER_10M_2021_V2</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>15 arcsec (463m @equator)</t>
+  </si>
+  <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>100m</t>
+  </si>
+  <si>
+    <t>30 arcsec (~1 km)</t>
+  </si>
+  <si>
+    <t>250m</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>PVOUT (kWh/kW/a)</t>
+  </si>
+  <si>
+    <t>wind speed @100m</t>
+  </si>
+  <si>
+    <t>actual DTM</t>
+  </si>
+  <si>
+    <t>not used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,13 +291,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,18 +329,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -615,80 +677,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18C1CA-23D3-47BC-BC83-CDCB1C3DDEFC}">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D31C76-1A8C-4B0E-AE4B-BACC3D2A9F3D}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D071E76A-CA52-41A0-A384-F19AC57A0B0C}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{D65E9C3A-1F86-43EA-8F2A-DDB67D1B7BF3}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{E8928AF7-5BD9-4484-921D-01DC3E921B47}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{3E840665-3C2E-4816-B118-F1DECECFD536}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{9A10D374-DFD4-43E5-942D-9058CD9EBFDE}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{6BE7D4DB-648A-445A-892D-9E8816FA8346}"/>
+    <hyperlink ref="B20" r:id="rId7" xr:uid="{0B617A10-23AA-4D90-8756-9D0680367E6B}"/>
+    <hyperlink ref="B19" r:id="rId8" xr:uid="{5AEB4E2A-2394-4A6D-A91F-B62BAFE90E18}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18C1CA-23D3-47BC-BC83-CDCB1C3DDEFC}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -696,357 +1022,291 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
       <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="D29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D92FEE-935E-421C-95F5-75F49D715FF2}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1054,278 +1314,520 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8C519A0C07EDA47BFE3C2D04A9A16E8" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5af8a87c7f5a09efbaa0de1bfbdabc53">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7" xmlns:ns3="730a4b66-01d8-4cde-8d8b-f146b54eaab0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d85c399567fc6e954f4786affeeee316" ns2:_="" ns3:_="">
+    <xsd:import namespace="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7"/>
+    <xsd:import namespace="730a4b66-01d8-4cde-8d8b-f146b54eaab0"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:_dlc_DocId" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdUrl" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdPersistId" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_dlc_DocId" ma:index="8" nillable="true" ma:displayName="Document ID Value" ma:description="The value of the document ID assigned to this item." ma:internalName="_dlc_DocId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdUrl" ma:index="9" nillable="true" ma:displayName="Document ID" ma:description="Permanent link to this document." ma:hidden="true" ma:internalName="_dlc_DocIdUrl" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdPersistId" ma:index="10" nillable="true" ma:displayName="Persist ID" ma:description="Keep ID on add." ma:hidden="true" ma:internalName="_dlc_DocIdPersistId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="730a4b66-01d8-4cde-8d8b-f146b54eaab0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7">GE00-939878155-298</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7">
+      <Url>https://sp.ens.dk/sites/gr/keny/_layouts/15/DocIdRedir.aspx?ID=GE00-939878155-298</Url>
+      <Description>GE00-939878155-298</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2FE42FC-3536-4A73-B9F7-AADAD56E28F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7"/>
+    <ds:schemaRef ds:uri="730a4b66-01d8-4cde-8d8b-f146b54eaab0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64FA2BBB-2582-437A-AF5D-6FFA5E5689E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{964EE766-D6F8-4013-8CB4-BEDD892B39AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD566AB5-C4C6-4641-BE27-5E6E12A6FDD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="730a4b66-01d8-4cde-8d8b-f146b54eaab0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e27f82ce-7993-4fa5-92ff-7ebb6bd1aea7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>